<commit_message>
Exi updates on text
</commit_message>
<xml_diff>
--- a/Tiago/Exi_Map Data.xlsx
+++ b/Tiago/Exi_Map Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\VM Shared Folder\Github\DataVis\DataVis2021\Tiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96CF317-DA59-4B67-AA9B-AB42EA567073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A09625-F63B-47E9-A8FD-1A4CBDC691A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14705,8 +14705,8 @@
   <dimension ref="A1:L179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J170" sqref="J170"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18404,9 +18404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98A65E5-9EDC-4BB6-B2A3-1DFF833E97F5}">
   <dimension ref="A1:AD167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE14" sqref="AE14"/>
+      <selection pane="bottomLeft" activeCell="AD7" sqref="AD7:AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25155,7 +25155,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>